<commit_message>
refactor(create-station): add station #
</commit_message>
<xml_diff>
--- a/forms/contact/station-create.xlsx
+++ b/forms/contact/station-create.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Work/dccms/daily-register/forms/contact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B7037-A03E-4F45-8F29-518E3517C9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B16E30A-455E-F344-86E0-17BBA9D2A653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="207">
   <si>
     <t>type</t>
   </si>
@@ -653,13 +653,19 @@
   </si>
   <si>
     <t>New Assistant</t>
+  </si>
+  <si>
+    <t>station_number</t>
+  </si>
+  <si>
+    <t>Station number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -683,6 +689,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -765,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -808,6 +820,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,13 +1204,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG21"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1598,38 +1612,35 @@
       </c>
     </row>
     <row r="14" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:33" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>204</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
-      </c>
-    </row>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:33" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>204</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1637,10 +1648,10 @@
         <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
@@ -1651,34 +1662,48 @@
         <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>202</v>
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>203</v>
-      </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2401,7 +2426,7 @@
       </c>
       <c r="C2" s="25" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-04-18 4-28</v>
+        <v>2023-06-27 15-32</v>
       </c>
       <c r="D2" t="s">
         <v>196</v>

</xml_diff>